<commit_message>
updated data, added TimeLagAnalysis script -KL
</commit_message>
<xml_diff>
--- a/DataUpdate/data/Testing_DataFrame.xlsx
+++ b/DataUpdate/data/Testing_DataFrame.xlsx
@@ -1332,7 +1332,7 @@
         <v>111</v>
       </c>
       <c r="T2">
-        <v>78.40195280866459</v>
+        <v>79.42851574123137</v>
       </c>
       <c r="U2">
         <v>20200508</v>
@@ -1478,7 +1478,7 @@
         <v>112</v>
       </c>
       <c r="T3">
-        <v>122.1512908712787</v>
+        <v>123.2952574732174</v>
       </c>
       <c r="U3">
         <v>20200508</v>
@@ -1627,7 +1627,7 @@
         <v>113</v>
       </c>
       <c r="T4">
-        <v>32.60188270765806</v>
+        <v>35.57619318654503</v>
       </c>
       <c r="U4">
         <v>20200508</v>
@@ -1794,7 +1794,7 @@
         <v>114</v>
       </c>
       <c r="T5">
-        <v>68.19546111693711</v>
+        <v>68.98063261057932</v>
       </c>
       <c r="U5">
         <v>20200508</v>
@@ -1949,7 +1949,7 @@
         <v>115</v>
       </c>
       <c r="T6">
-        <v>71.46093423817067</v>
+        <v>71.93161907612469</v>
       </c>
       <c r="U6">
         <v>20200508</v>
@@ -2101,7 +2101,7 @@
         <v>116</v>
       </c>
       <c r="T7">
-        <v>40.70602704274426</v>
+        <v>41.25751180954379</v>
       </c>
       <c r="U7">
         <v>20200508</v>
@@ -2256,7 +2256,7 @@
         <v>117</v>
       </c>
       <c r="T8">
-        <v>85.13196898355658</v>
+        <v>85.5818596394662</v>
       </c>
       <c r="U8">
         <v>20200508</v>
@@ -2405,7 +2405,7 @@
         <v>118</v>
       </c>
       <c r="T9">
-        <v>65.11074865671625</v>
+        <v>66.29500823011963</v>
       </c>
       <c r="U9">
         <v>20200508</v>
@@ -2548,7 +2548,7 @@
         <v>119</v>
       </c>
       <c r="T10">
-        <v>88.86513975318897</v>
+        <v>90.65587845786484</v>
       </c>
       <c r="U10">
         <v>20200508</v>
@@ -2706,7 +2706,7 @@
         <v>120</v>
       </c>
       <c r="T11">
-        <v>58.68636227796307</v>
+        <v>59.38041122973839</v>
       </c>
       <c r="U11">
         <v>20200508</v>
@@ -2852,7 +2852,7 @@
         <v>121</v>
       </c>
       <c r="T12">
-        <v>65.99468950421037</v>
+        <v>67.24773137727452</v>
       </c>
       <c r="U12">
         <v>20200508</v>
@@ -3001,7 +3001,7 @@
         <v>122</v>
       </c>
       <c r="T13">
-        <v>49.52710383067416</v>
+        <v>49.04403004832292</v>
       </c>
       <c r="U13">
         <v>20200508</v>
@@ -3150,7 +3150,7 @@
         <v>123</v>
       </c>
       <c r="T14">
-        <v>47.02201595395449</v>
+        <v>46.67766993614866</v>
       </c>
       <c r="U14">
         <v>20200508</v>
@@ -3293,7 +3293,7 @@
         <v>124</v>
       </c>
       <c r="T15">
-        <v>98.79969506008784</v>
+        <v>100.9536687017665</v>
       </c>
       <c r="U15">
         <v>20200508</v>
@@ -3448,7 +3448,7 @@
         <v>125</v>
       </c>
       <c r="T16">
-        <v>51.15241344880124</v>
+        <v>52.01816211634516</v>
       </c>
       <c r="U16">
         <v>20200508</v>
@@ -3609,7 +3609,7 @@
         <v>126</v>
       </c>
       <c r="T17">
-        <v>74.93976043797605</v>
+        <v>76.86563734451821</v>
       </c>
       <c r="U17">
         <v>20200508</v>
@@ -3770,7 +3770,7 @@
         <v>127</v>
       </c>
       <c r="T18">
-        <v>52.49229502106128</v>
+        <v>54.18419287058687</v>
       </c>
       <c r="U18">
         <v>20200508</v>
@@ -3925,7 +3925,7 @@
         <v>128</v>
       </c>
       <c r="T19">
-        <v>56.37853080856946</v>
+        <v>59.51531127249995</v>
       </c>
       <c r="U19">
         <v>20200508</v>
@@ -4083,7 +4083,7 @@
         <v>129</v>
       </c>
       <c r="T20">
-        <v>70.69805522872079</v>
+        <v>73.15315572356192</v>
       </c>
       <c r="U20">
         <v>20200508</v>
@@ -4238,7 +4238,7 @@
         <v>130</v>
       </c>
       <c r="T21">
-        <v>39.38176826768373</v>
+        <v>39.02044398478295</v>
       </c>
       <c r="U21">
         <v>20200508</v>
@@ -4405,7 +4405,7 @@
         <v>131</v>
       </c>
       <c r="T22">
-        <v>70.45450702074143</v>
+        <v>70.70041955415016</v>
       </c>
       <c r="U22">
         <v>20200508</v>
@@ -4563,7 +4563,7 @@
         <v>132</v>
       </c>
       <c r="T23">
-        <v>145.5326236458054</v>
+        <v>146.4679487280519</v>
       </c>
       <c r="U23">
         <v>20200508</v>
@@ -4715,7 +4715,7 @@
         <v>133</v>
       </c>
       <c r="T24">
-        <v>86.89258457489262</v>
+        <v>88.98555492173882</v>
       </c>
       <c r="U24">
         <v>20200508</v>
@@ -4876,7 +4876,7 @@
         <v>134</v>
       </c>
       <c r="T25">
-        <v>49.41604977236012</v>
+        <v>50.98030365658955</v>
       </c>
       <c r="U25">
         <v>20200508</v>
@@ -5040,7 +5040,7 @@
         <v>135</v>
       </c>
       <c r="T26">
-        <v>75.4094898026222</v>
+        <v>73.67547077190636</v>
       </c>
       <c r="U26">
         <v>20200508</v>
@@ -5198,7 +5198,7 @@
         <v>136</v>
       </c>
       <c r="T27">
-        <v>39.9258623907254</v>
+        <v>40.73555247053601</v>
       </c>
       <c r="U27">
         <v>20200508</v>
@@ -5350,7 +5350,7 @@
         <v>137</v>
       </c>
       <c r="T28">
-        <v>44.15734016690813</v>
+        <v>46.71267873852356</v>
       </c>
       <c r="U28">
         <v>20200508</v>
@@ -5496,7 +5496,7 @@
         <v>138</v>
       </c>
       <c r="T29">
-        <v>73.78043121846544</v>
+        <v>76.35929319148482</v>
       </c>
       <c r="U29">
         <v>20200508</v>
@@ -5630,7 +5630,7 @@
         <v>139</v>
       </c>
       <c r="T30">
-        <v>34.30471647877099</v>
+        <v>35.30276851946299</v>
       </c>
       <c r="U30">
         <v>20200508</v>
@@ -5773,7 +5773,7 @@
         <v>140</v>
       </c>
       <c r="T31">
-        <v>58.41122719680475</v>
+        <v>59.84841139159953</v>
       </c>
       <c r="U31">
         <v>20200508</v>
@@ -5928,7 +5928,7 @@
         <v>141</v>
       </c>
       <c r="T32">
-        <v>77.87486289712206</v>
+        <v>77.4295813193125</v>
       </c>
       <c r="U32">
         <v>20200508</v>
@@ -6092,7 +6092,7 @@
         <v>142</v>
       </c>
       <c r="T33">
-        <v>145.676475166514</v>
+        <v>148.0919216512835</v>
       </c>
       <c r="U33">
         <v>20200508</v>
@@ -6247,7 +6247,7 @@
         <v>143</v>
       </c>
       <c r="T34">
-        <v>151.5333516995682</v>
+        <v>152.6006981941599</v>
       </c>
       <c r="U34">
         <v>20200508</v>
@@ -6405,7 +6405,7 @@
         <v>144</v>
       </c>
       <c r="T35">
-        <v>44.61553204038288</v>
+        <v>45.8292545256063</v>
       </c>
       <c r="U35">
         <v>20200508</v>
@@ -6551,7 +6551,7 @@
         <v>145</v>
       </c>
       <c r="T36">
-        <v>209.5559669715727</v>
+        <v>214.3355849597693</v>
       </c>
       <c r="U36">
         <v>20200508</v>
@@ -6703,7 +6703,7 @@
         <v>146</v>
       </c>
       <c r="T37">
-        <v>40.84023796119701</v>
+        <v>42.0482411963317</v>
       </c>
       <c r="U37">
         <v>20200508</v>
@@ -6870,7 +6870,7 @@
         <v>147</v>
       </c>
       <c r="T38">
-        <v>65.23369391298398</v>
+        <v>67.36765891228413</v>
       </c>
       <c r="U38">
         <v>20200508</v>
@@ -7031,7 +7031,7 @@
         <v>148</v>
       </c>
       <c r="T39">
-        <v>40.5140042187868</v>
+        <v>41.09569937623688</v>
       </c>
       <c r="U39">
         <v>20200508</v>
@@ -7189,7 +7189,7 @@
         <v>149</v>
       </c>
       <c r="T40">
-        <v>45.08843087894125</v>
+        <v>45.3343464284967</v>
       </c>
       <c r="U40">
         <v>20200508</v>
@@ -7341,7 +7341,7 @@
         <v>150</v>
       </c>
       <c r="T41">
-        <v>241.9978890688336</v>
+        <v>242.7265399639927</v>
       </c>
       <c r="U41">
         <v>20200508</v>
@@ -7508,7 +7508,7 @@
         <v>151</v>
       </c>
       <c r="T42">
-        <v>34.46898699369738</v>
+        <v>35.40435868230194</v>
       </c>
       <c r="U42">
         <v>20200508</v>
@@ -7657,7 +7657,7 @@
         <v>152</v>
       </c>
       <c r="T43">
-        <v>63.56393394216563</v>
+        <v>65.13417548341353</v>
       </c>
       <c r="U43">
         <v>20200508</v>
@@ -7812,7 +7812,7 @@
         <v>153</v>
       </c>
       <c r="T44">
-        <v>105.3745679218503</v>
+        <v>106.6127349756764</v>
       </c>
       <c r="U44">
         <v>20200508</v>
@@ -7955,7 +7955,7 @@
         <v>154</v>
       </c>
       <c r="T45">
-        <v>59.35348237693893</v>
+        <v>60.1188685680356</v>
       </c>
       <c r="U45">
         <v>20200508</v>
@@ -8104,7 +8104,7 @@
         <v>155</v>
       </c>
       <c r="T46">
-        <v>135.930617911748</v>
+        <v>135.8350386123793</v>
       </c>
       <c r="U46">
         <v>20200508</v>
@@ -8259,7 +8259,7 @@
         <v>156</v>
       </c>
       <c r="T47">
-        <v>53.18442562087461</v>
+        <v>53.86402500069548</v>
       </c>
       <c r="U47">
         <v>20200508</v>
@@ -8408,7 +8408,7 @@
         <v>157</v>
       </c>
       <c r="T48">
-        <v>44.94855457853617</v>
+        <v>45.89301057888606</v>
       </c>
       <c r="U48">
         <v>20200508</v>
@@ -8569,7 +8569,7 @@
         <v>158</v>
       </c>
       <c r="T49">
-        <v>68.62905913058393</v>
+        <v>68.59910919115021</v>
       </c>
       <c r="U49">
         <v>20200508</v>
@@ -8715,7 +8715,7 @@
         <v>159</v>
       </c>
       <c r="T50">
-        <v>142.1645803135348</v>
+        <v>141.9424880444684</v>
       </c>
       <c r="U50">
         <v>20200508</v>
@@ -8876,7 +8876,7 @@
         <v>160</v>
       </c>
       <c r="T51">
-        <v>48.90238051569887</v>
+        <v>50.41423878759534</v>
       </c>
       <c r="U51">
         <v>20200508</v>
@@ -9043,7 +9043,7 @@
         <v>161</v>
       </c>
       <c r="T52">
-        <v>48.77792324574818</v>
+        <v>49.09888572951384</v>
       </c>
       <c r="U52">
         <v>20200508</v>

</xml_diff>